<commit_message>
Update Excel list with country-wise notes on Shapefile versions
</commit_message>
<xml_diff>
--- a/obs-pop-figures-shapes.xlsx
+++ b/obs-pop-figures-shapes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakobarendt/Documents/r-projects/mathesis-depop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15E252B-32E7-454F-BBFA-8EF9BB85138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6151EF32-D598-B842-ABFE-07A110653FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21220" yWindow="500" windowWidth="29980" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>CNTR_CODE</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>cannot join</t>
+  </si>
+  <si>
+    <t>no diff for ID</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,6 +248,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +559,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -605,7 +612,7 @@
       <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -625,6 +632,9 @@
       <c r="E3" t="s">
         <v>40</v>
       </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -837,7 +847,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B16">
@@ -856,7 +866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -872,8 +882,8 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B18">
@@ -892,7 +902,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -909,7 +919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -923,7 +933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -943,8 +953,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B22">
@@ -963,8 +973,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B23">
@@ -980,7 +990,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -997,7 +1007,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1013,8 +1023,11 @@
       <c r="E25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1031,7 +1044,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1045,13 +1058,13 @@
         <v>426</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1065,13 +1078,13 @@
         <v>2478</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -1088,7 +1101,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1104,8 +1117,11 @@
       <c r="E30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1121,8 +1137,11 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>34</v>
       </c>
@@ -1139,7 +1158,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1155,8 +1174,11 @@
       <c r="E33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
@@ -1168,7 +1190,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>

</xml_diff>